<commit_message>
updated salinity data + re ran script
</commit_message>
<xml_diff>
--- a/airica/data/LD_storage_test/AIRICA_storage_test.xlsx
+++ b/airica/data/LD_storage_test/AIRICA_storage_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\lab-work\airica\data\LD_storage_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7B7241-6A5C-4D4B-BEE1-D33802A2CE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BB86A8-D165-4FAA-BC77-55C95D7A0329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{7741F939-3579-4835-AC9B-056E5DC56150}"/>
   </bookViews>
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD63930-A9D0-4326-B92B-8C89864D4982}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="U27" sqref="U27:V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +806,7 @@
         <v>4</v>
       </c>
       <c r="U2" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V2" s="1">
         <v>-9999</v>
@@ -884,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="U3" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V3" s="1">
         <v>306.60000000000002</v>
@@ -960,7 +960,7 @@
         <v>2</v>
       </c>
       <c r="U4" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V4" s="1">
         <v>308.39999999999998</v>
@@ -1038,7 +1038,7 @@
         <v>2</v>
       </c>
       <c r="U5" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V5" s="1">
         <v>308.60000000000002</v>
@@ -1114,7 +1114,7 @@
         <v>2</v>
       </c>
       <c r="U6" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V6" s="1">
         <v>3270.1</v>
@@ -1192,7 +1192,7 @@
         <v>2</v>
       </c>
       <c r="U7" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V7" s="1">
         <v>3270.8</v>
@@ -1268,7 +1268,7 @@
         <v>4</v>
       </c>
       <c r="U8" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V8" s="1">
         <v>-9999</v>
@@ -1574,7 +1574,7 @@
         <v>2</v>
       </c>
       <c r="U12" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V12" s="1">
         <v>3277.8</v>
@@ -1652,7 +1652,7 @@
         <v>2</v>
       </c>
       <c r="U13" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V13" s="1">
         <v>3277.2</v>
@@ -1728,7 +1728,7 @@
         <v>2</v>
       </c>
       <c r="U14" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V14" s="1">
         <v>3281.3</v>
@@ -1804,7 +1804,7 @@
         <v>2</v>
       </c>
       <c r="U15" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V15" s="1">
         <v>3277.9</v>
@@ -1880,7 +1880,7 @@
         <v>2</v>
       </c>
       <c r="U16" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V16" s="1">
         <v>3280.2</v>
@@ -1956,7 +1956,7 @@
         <v>2</v>
       </c>
       <c r="U17" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V17" s="1">
         <v>3274.2</v>
@@ -2032,7 +2032,7 @@
         <v>2</v>
       </c>
       <c r="U18" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V18" s="1">
         <v>3270.5</v>
@@ -2108,7 +2108,7 @@
         <v>2</v>
       </c>
       <c r="U19" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V19" s="1">
         <v>3271.3</v>
@@ -2183,7 +2183,7 @@
         <v>2</v>
       </c>
       <c r="U20" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V20" s="1">
         <v>3272.7</v>
@@ -2258,7 +2258,7 @@
         <v>2</v>
       </c>
       <c r="U21" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V21" s="1">
         <v>3272.9</v>

</xml_diff>

<commit_message>
added new DIC data
</commit_message>
<xml_diff>
--- a/airica/data/LD_storage_test/AIRICA_storage_test.xlsx
+++ b/airica/data/LD_storage_test/AIRICA_storage_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\lab-work\airica\data\LD_storage_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BB86A8-D165-4FAA-BC77-55C95D7A0329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A9909D-B646-4BBC-821D-DECD3321140C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{7741F939-3579-4835-AC9B-056E5DC56150}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{7741F939-3579-4835-AC9B-056E5DC56150}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="140">
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>CV%</t>
+  </si>
   <si>
     <t>Notes</t>
   </si>
@@ -81,9 +87,6 @@
     <t>Weird calculations - restarting system but NOT "reset zero" for Li-cor (restarted after J03)</t>
   </si>
   <si>
-    <t>RESET ZERO before J05 + changed CALCULATION MODE to "reject first" (aoso before running J05)</t>
-  </si>
-  <si>
     <t>Aborted - pressed wrong button</t>
   </si>
   <si>
@@ -108,9 +111,18 @@
     <t>U49</t>
   </si>
   <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
     <t>U06</t>
   </si>
   <si>
+    <t>CRM-189-0099-1200-2</t>
+  </si>
+  <si>
     <t>R17</t>
   </si>
   <si>
@@ -120,16 +132,136 @@
     <t>U02</t>
   </si>
   <si>
+    <t>CRM-189-0099-1200-3</t>
+  </si>
+  <si>
+    <t>13/10/2021</t>
+  </si>
+  <si>
+    <t>J08</t>
+  </si>
+  <si>
+    <t>J09</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>Restarted laptop + Licor before this one</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>Restarted software before this one</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>no name</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>Pressed without selecting sample in sample list</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>J16</t>
+  </si>
+  <si>
+    <t>J17</t>
+  </si>
+  <si>
+    <t>CRM-189-0102-1000</t>
+  </si>
+  <si>
+    <t>replicate #2 - subsampled from 500 mL bottle</t>
+  </si>
+  <si>
+    <t>CRM-189-0102-1200</t>
+  </si>
+  <si>
+    <t>replicate #4 - subsampled from 500 mL bottle</t>
+  </si>
+  <si>
+    <t>CRM-189-0102-1400</t>
+  </si>
+  <si>
+    <t>replicate #9 - subsampled from 500 mL bottle</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>U45</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>U35</t>
+  </si>
+  <si>
+    <t>U25</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>RESET ZERO before J05 + changed CALCULATION MODE to "reject first" (also before running J05)</t>
+  </si>
+  <si>
+    <t>analysis_batch</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
+    <t>measurement_time</t>
+  </si>
+  <si>
+    <t>analysis_date</t>
+  </si>
+  <si>
+    <t>pre_acid_time</t>
+  </si>
+  <si>
+    <t>post_acid_tiem</t>
+  </si>
+  <si>
+    <t>extra_time</t>
+  </si>
+  <si>
     <t>sample_v</t>
   </si>
   <si>
     <t>rinsing_v</t>
   </si>
   <si>
-    <t>filling_peed</t>
+    <t>filling_speed</t>
   </si>
   <si>
     <t>rinsing_speed</t>
@@ -147,145 +279,191 @@
     <t>rinsing_mode</t>
   </si>
   <si>
+    <t>rinse_for_replicates</t>
+  </si>
+  <si>
+    <t>database_name</t>
+  </si>
+  <si>
     <t>all_to_stripped</t>
   </si>
   <si>
-    <t>rinse_for_replicates</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
-    <t>database_name</t>
-  </si>
-  <si>
     <t>LD_storage_test.dbs</t>
   </si>
   <si>
     <t>filename</t>
   </si>
   <si>
+    <t>0-0  0  (0)J01.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J02.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J03.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J04.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J05.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J06.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J07.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)CRM-189-0099-1000.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)CRM-189-0099-1200.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)CRM-189-0099-1400.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)R13.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)R20.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)U14.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)U42.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)R12.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)U49.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)U06.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)R17.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)R08.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)U02.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)CRM-189-0099-2.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)CRM-189-0099-3.dat</t>
+  </si>
+  <si>
     <t>flag</t>
   </si>
   <si>
-    <t>0-0  0  (0)J01.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)J02.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)J03.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)J04.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)J05.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)J06.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)J07.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)CRM-189-0099-1000.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)CRM-189-0099-1200.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)CRM-189-0099-1400.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)CRM-189-0099-2.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)CRM-189-0099-3.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)R13.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)R20.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)U14.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)U42.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)R12.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)U49.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)U06.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)R17.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)R08.dat</t>
-  </si>
-  <si>
-    <t>0-0  0  (0)U02.dat</t>
-  </si>
-  <si>
-    <t>analysis_batch</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>cv%</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>CRM</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>measurement_time</t>
-  </si>
-  <si>
-    <t>pre_acid_time</t>
-  </si>
-  <si>
-    <t>post_acid_tiem</t>
-  </si>
-  <si>
-    <t>extra_time</t>
-  </si>
-  <si>
     <t>salinity</t>
   </si>
   <si>
-    <t>CRM-189-0099-2</t>
-  </si>
-  <si>
-    <t>CRM-189-0099-3</t>
+    <t>0-0  0  (0)J08.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J09.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J10.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J15.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J16.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J17.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)CRM-189-0102-1000.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)CRM-189-0102-1200.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)CRM-189-0102-1400.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)R38.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J1.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J12.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J13.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)J14.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)R10.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)U45.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)R31.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)U35.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)U25.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)R21.dat</t>
+  </si>
+  <si>
+    <t>U01</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)U01.dat</t>
+  </si>
+  <si>
+    <t>U32</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)U32.dat</t>
+  </si>
+  <si>
+    <t>R46</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)R46.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)CRM-189-0102-1200-2.dat</t>
+  </si>
+  <si>
+    <t>replicate #3 - subsampled from 500 mL bottle</t>
+  </si>
+  <si>
+    <t>CRM-189-0102-1200-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -329,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -337,7 +515,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -654,107 +844,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD63930-A9D0-4326-B92B-8C89864D4982}">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27:V27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="12.5703125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="8.7109375" style="1"/>
+    <col min="5" max="18" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" style="1" customWidth="1"/>
+    <col min="20" max="21" width="8.7109375" style="1"/>
+    <col min="22" max="22" width="8.7109375" style="3"/>
+    <col min="23" max="23" width="8.7109375" style="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="N1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="U1" s="3" t="s">
+      <c r="O1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y1" s="3" t="s">
+      <c r="P1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>0</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1">
         <v>360</v>
@@ -775,13 +973,12 @@
         <v>1200</v>
       </c>
       <c r="K2" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L2" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M2" s="1">
-        <f>L2/100</f>
         <v>18</v>
       </c>
       <c r="N2" s="1">
@@ -791,48 +988,48 @@
         <v>2</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="T2" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="U2" s="1">
         <v>32</v>
       </c>
-      <c r="V2" s="1">
+      <c r="V2" s="7">
         <v>-9999</v>
       </c>
       <c r="W2" s="1">
         <v>-9999</v>
       </c>
-      <c r="X2" s="1">
+      <c r="X2" s="7">
         <v>-9999</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1">
         <v>360</v>
@@ -853,13 +1050,12 @@
         <v>1200</v>
       </c>
       <c r="K3" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L3" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M23" si="0">L3/100</f>
         <v>18</v>
       </c>
       <c r="N3" s="1">
@@ -869,46 +1065,46 @@
         <v>2</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="T3" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="U3" s="1">
         <v>32</v>
       </c>
-      <c r="V3" s="1">
+      <c r="V3" s="3">
         <v>306.60000000000002</v>
       </c>
       <c r="W3" s="1">
         <v>22830</v>
       </c>
-      <c r="X3" s="1">
+      <c r="X3" s="4">
         <v>0.61</v>
       </c>
       <c r="Y3" s="2"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1">
         <v>360</v>
@@ -929,13 +1125,12 @@
         <v>1200</v>
       </c>
       <c r="K4" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L4" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N4" s="1">
@@ -945,48 +1140,48 @@
         <v>2</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="T4" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="U4" s="1">
         <v>32</v>
       </c>
-      <c r="V4" s="1">
+      <c r="V4" s="3">
         <v>308.39999999999998</v>
       </c>
       <c r="W4" s="1">
         <v>22966</v>
       </c>
-      <c r="X4" s="1">
+      <c r="X4" s="4">
         <v>0.113</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1">
         <v>360</v>
@@ -1007,13 +1202,12 @@
         <v>1200</v>
       </c>
       <c r="K5" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L5" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N5" s="1">
@@ -1023,46 +1217,46 @@
         <v>2</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="T5" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="U5" s="1">
         <v>32</v>
       </c>
-      <c r="V5" s="1">
+      <c r="V5" s="3">
         <v>308.60000000000002</v>
       </c>
       <c r="W5" s="1">
         <v>22977</v>
       </c>
-      <c r="X5" s="1">
+      <c r="X5" s="4">
         <v>0.214</v>
       </c>
       <c r="Y5" s="2"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1">
         <v>360</v>
@@ -1083,13 +1277,12 @@
         <v>1200</v>
       </c>
       <c r="K6" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L6" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N6" s="1">
@@ -1099,124 +1292,123 @@
         <v>2</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="T6" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="U6" s="1">
         <v>32</v>
       </c>
-      <c r="V6" s="1">
+      <c r="V6" s="3">
         <v>3270.1</v>
       </c>
       <c r="W6" s="1">
         <v>24347</v>
       </c>
-      <c r="X6" s="1">
+      <c r="X6" s="4">
         <v>0.08</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>360</v>
+      </c>
+      <c r="F7" s="1">
+        <v>75</v>
+      </c>
+      <c r="G7" s="1">
+        <v>120</v>
+      </c>
+      <c r="H7" s="1">
+        <v>10</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K7" s="1">
+        <v>150</v>
+      </c>
+      <c r="L7" s="1">
+        <v>150</v>
+      </c>
+      <c r="M7" s="1">
+        <v>18</v>
+      </c>
+      <c r="N7" s="1">
+        <v>3</v>
+      </c>
+      <c r="O7" s="1">
+        <v>2</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="T7" s="1">
         <v>7</v>
-      </c>
-      <c r="E7" s="1">
-        <v>360</v>
-      </c>
-      <c r="F7" s="1">
-        <v>75</v>
-      </c>
-      <c r="G7" s="1">
-        <v>120</v>
-      </c>
-      <c r="H7" s="1">
-        <v>10</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1200</v>
-      </c>
-      <c r="J7" s="1">
-        <v>1200</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1800</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1800</v>
-      </c>
-      <c r="M7" s="1">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="N7" s="1">
-        <v>3</v>
-      </c>
-      <c r="O7" s="1">
-        <v>2</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T7" s="1">
-        <v>2</v>
       </c>
       <c r="U7" s="1">
         <v>32</v>
       </c>
-      <c r="V7" s="1">
+      <c r="V7" s="3">
         <v>3270.8</v>
       </c>
       <c r="W7" s="1">
         <v>24353</v>
       </c>
-      <c r="X7" s="1">
+      <c r="X7" s="4">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="Y7" s="2"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1">
         <v>360</v>
@@ -1237,13 +1429,12 @@
         <v>1200</v>
       </c>
       <c r="K8" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L8" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N8" s="1">
@@ -1253,48 +1444,48 @@
         <v>2</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="T8" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="U8" s="1">
         <v>32</v>
       </c>
-      <c r="V8" s="1">
+      <c r="V8" s="7">
         <v>-9999</v>
       </c>
       <c r="W8" s="1">
         <v>-9999</v>
       </c>
-      <c r="X8" s="1">
+      <c r="X8" s="7">
         <v>-9999</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1">
         <v>360</v>
@@ -1315,13 +1506,12 @@
         <v>1000</v>
       </c>
       <c r="K9" s="1">
-        <v>1500</v>
+        <v>150</v>
       </c>
       <c r="L9" s="1">
-        <v>1500</v>
+        <v>150</v>
       </c>
       <c r="M9" s="1">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="N9" s="1">
@@ -1331,16 +1521,16 @@
         <v>2</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="T9" s="1">
         <v>2</v>
@@ -1348,29 +1538,29 @@
       <c r="U9" s="1">
         <v>33.494</v>
       </c>
-      <c r="V9" s="1">
+      <c r="V9" s="3">
         <v>3033.2</v>
       </c>
       <c r="W9" s="1">
         <v>18819</v>
       </c>
-      <c r="X9" s="1">
+      <c r="X9" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="Y9" s="2"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1">
         <v>360</v>
@@ -1391,13 +1581,12 @@
         <v>1200</v>
       </c>
       <c r="K10" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L10" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M10" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N10" s="1">
@@ -1407,16 +1596,16 @@
         <v>2</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="T10" s="1">
         <v>2</v>
@@ -1424,29 +1613,29 @@
       <c r="U10" s="1">
         <v>33.494</v>
       </c>
-      <c r="V10" s="1">
+      <c r="V10" s="3">
         <v>3041.8</v>
       </c>
       <c r="W10" s="1">
         <v>22647</v>
       </c>
-      <c r="X10" s="1">
+      <c r="X10" s="4">
         <v>0.06</v>
       </c>
       <c r="Y10" s="2"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1">
         <v>360</v>
@@ -1467,13 +1656,12 @@
         <v>1400</v>
       </c>
       <c r="K11" s="1">
-        <v>2100</v>
+        <v>150</v>
       </c>
       <c r="L11" s="1">
-        <v>2100</v>
+        <v>150</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="N11" s="1">
@@ -1483,16 +1671,16 @@
         <v>2</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="T11" s="1">
         <v>2</v>
@@ -1500,29 +1688,29 @@
       <c r="U11" s="1">
         <v>33.494</v>
       </c>
-      <c r="V11" s="1">
+      <c r="V11" s="3">
         <v>3038.3</v>
       </c>
       <c r="W11" s="1">
         <v>26391</v>
       </c>
-      <c r="X11" s="1">
+      <c r="X11" s="4">
         <v>0.24299999999999999</v>
       </c>
       <c r="Y11" s="2"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E12" s="1">
         <v>360</v>
@@ -1543,13 +1731,12 @@
         <v>1200</v>
       </c>
       <c r="K12" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L12" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N12" s="1">
@@ -1559,16 +1746,16 @@
         <v>2</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="T12" s="1">
         <v>2</v>
@@ -1576,60 +1763,59 @@
       <c r="U12" s="1">
         <v>32</v>
       </c>
-      <c r="V12" s="1">
+      <c r="V12" s="3">
         <v>3277.8</v>
       </c>
       <c r="W12" s="1">
         <v>24404</v>
       </c>
-      <c r="X12" s="1">
+      <c r="X12" s="4">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1">
+        <v>360</v>
+      </c>
+      <c r="F13" s="1">
+        <v>75</v>
+      </c>
+      <c r="G13" s="1">
+        <v>120</v>
+      </c>
+      <c r="H13" s="1">
+        <v>10</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K13" s="1">
+        <v>150</v>
+      </c>
+      <c r="L13" s="1">
+        <v>150</v>
+      </c>
+      <c r="M13" s="1">
         <v>18</v>
       </c>
-      <c r="E13" s="1">
-        <v>360</v>
-      </c>
-      <c r="F13" s="1">
-        <v>75</v>
-      </c>
-      <c r="G13" s="1">
-        <v>120</v>
-      </c>
-      <c r="H13" s="1">
-        <v>10</v>
-      </c>
-      <c r="I13" s="1">
-        <v>1200</v>
-      </c>
-      <c r="J13" s="1">
-        <v>1200</v>
-      </c>
-      <c r="K13" s="1">
-        <v>1800</v>
-      </c>
-      <c r="L13" s="1">
-        <v>1800</v>
-      </c>
-      <c r="M13" s="1">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
       <c r="N13" s="1">
         <v>3</v>
       </c>
@@ -1637,16 +1823,16 @@
         <v>2</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="T13" s="1">
         <v>2</v>
@@ -1654,29 +1840,29 @@
       <c r="U13" s="1">
         <v>32</v>
       </c>
-      <c r="V13" s="1">
+      <c r="V13" s="3">
         <v>3277.2</v>
       </c>
       <c r="W13" s="1">
         <v>24399</v>
       </c>
-      <c r="X13" s="1">
+      <c r="X13" s="4">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="Y13" s="2"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" s="1">
         <v>360</v>
@@ -1697,13 +1883,12 @@
         <v>1200</v>
       </c>
       <c r="K14" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L14" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N14" s="1">
@@ -1713,16 +1898,16 @@
         <v>2</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="T14" s="1">
         <v>2</v>
@@ -1730,29 +1915,29 @@
       <c r="U14" s="1">
         <v>32</v>
       </c>
-      <c r="V14" s="1">
+      <c r="V14" s="3">
         <v>3281.3</v>
       </c>
       <c r="W14" s="1">
         <v>24428</v>
       </c>
-      <c r="X14" s="1">
+      <c r="X14" s="4">
         <v>0.05</v>
       </c>
       <c r="Y14" s="2"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E15" s="1">
         <v>360</v>
@@ -1773,13 +1958,12 @@
         <v>1200</v>
       </c>
       <c r="K15" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L15" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N15" s="1">
@@ -1789,16 +1973,16 @@
         <v>2</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="T15" s="1">
         <v>2</v>
@@ -1806,29 +1990,29 @@
       <c r="U15" s="1">
         <v>32</v>
       </c>
-      <c r="V15" s="1">
+      <c r="V15" s="3">
         <v>3277.9</v>
       </c>
       <c r="W15" s="1">
         <v>24402</v>
       </c>
-      <c r="X15" s="1">
+      <c r="X15" s="4">
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="Y15" s="2"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1">
         <v>360</v>
@@ -1849,13 +2033,12 @@
         <v>1200</v>
       </c>
       <c r="K16" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L16" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M16" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N16" s="1">
@@ -1865,16 +2048,16 @@
         <v>2</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="T16" s="1">
         <v>2</v>
@@ -1882,29 +2065,29 @@
       <c r="U16" s="1">
         <v>32</v>
       </c>
-      <c r="V16" s="1">
+      <c r="V16" s="3">
         <v>3280.2</v>
       </c>
       <c r="W16" s="1">
         <v>24420</v>
       </c>
-      <c r="X16" s="1">
+      <c r="X16" s="4">
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="Y16" s="2"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1">
         <v>360</v>
@@ -1925,13 +2108,12 @@
         <v>1200</v>
       </c>
       <c r="K17" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L17" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M17" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N17" s="1">
@@ -1941,16 +2123,16 @@
         <v>2</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="T17" s="1">
         <v>2</v>
@@ -1958,29 +2140,29 @@
       <c r="U17" s="1">
         <v>32</v>
       </c>
-      <c r="V17" s="1">
+      <c r="V17" s="3">
         <v>3274.2</v>
       </c>
       <c r="W17" s="1">
         <v>24374</v>
       </c>
-      <c r="X17" s="1">
+      <c r="X17" s="4">
         <v>5.5E-2</v>
       </c>
       <c r="Y17" s="2"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1">
         <v>360</v>
@@ -2001,13 +2183,12 @@
         <v>1200</v>
       </c>
       <c r="K18" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L18" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N18" s="1">
@@ -2017,16 +2198,16 @@
         <v>2</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="T18" s="1">
         <v>2</v>
@@ -2034,29 +2215,29 @@
       <c r="U18" s="1">
         <v>32</v>
       </c>
-      <c r="V18" s="1">
+      <c r="V18" s="3">
         <v>3270.5</v>
       </c>
       <c r="W18" s="1">
         <v>24350</v>
       </c>
-      <c r="X18" s="1">
+      <c r="X18" s="4">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="Y18" s="2"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E19" s="1">
         <v>360</v>
@@ -2077,13 +2258,12 @@
         <v>1200</v>
       </c>
       <c r="K19" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L19" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N19" s="1">
@@ -2093,16 +2273,16 @@
         <v>2</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="T19" s="1">
         <v>2</v>
@@ -2110,28 +2290,28 @@
       <c r="U19" s="1">
         <v>32</v>
       </c>
-      <c r="V19" s="1">
+      <c r="V19" s="3">
         <v>3271.3</v>
       </c>
       <c r="W19" s="1">
         <v>24553</v>
       </c>
-      <c r="X19" s="1">
+      <c r="X19" s="4">
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E20" s="1">
         <v>360</v>
@@ -2152,13 +2332,12 @@
         <v>1200</v>
       </c>
       <c r="K20" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L20" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M20" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N20" s="1">
@@ -2168,16 +2347,16 @@
         <v>2</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="T20" s="1">
         <v>2</v>
@@ -2185,28 +2364,28 @@
       <c r="U20" s="1">
         <v>32</v>
       </c>
-      <c r="V20" s="1">
+      <c r="V20" s="3">
         <v>3272.7</v>
       </c>
       <c r="W20" s="1">
         <v>24363</v>
       </c>
-      <c r="X20" s="1">
+      <c r="X20" s="4">
         <v>0.11600000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E21" s="1">
         <v>360</v>
@@ -2227,13 +2406,12 @@
         <v>1200</v>
       </c>
       <c r="K21" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L21" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N21" s="1">
@@ -2243,16 +2421,16 @@
         <v>2</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="T21" s="1">
         <v>2</v>
@@ -2260,28 +2438,28 @@
       <c r="U21" s="1">
         <v>32</v>
       </c>
-      <c r="V21" s="1">
+      <c r="V21" s="3">
         <v>3272.9</v>
       </c>
       <c r="W21" s="1">
         <v>24365</v>
       </c>
-      <c r="X21" s="1">
+      <c r="X21" s="4">
         <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="E22" s="1">
         <v>360</v>
@@ -2302,13 +2480,12 @@
         <v>1200</v>
       </c>
       <c r="K22" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L22" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N22" s="1">
@@ -2318,16 +2495,16 @@
         <v>2</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="T22" s="1">
         <v>2</v>
@@ -2335,28 +2512,28 @@
       <c r="U22" s="1">
         <v>33.494</v>
       </c>
-      <c r="V22" s="1">
+      <c r="V22" s="3">
         <v>3038.3</v>
       </c>
       <c r="W22" s="1">
         <v>22619</v>
       </c>
-      <c r="X22" s="1">
+      <c r="X22" s="4">
         <v>0.14799999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="E23" s="1">
         <v>360</v>
@@ -2377,13 +2554,12 @@
         <v>1200</v>
       </c>
       <c r="K23" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="L23" s="1">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="N23" s="1">
@@ -2393,16 +2569,16 @@
         <v>2</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="T23" s="1">
         <v>2</v>
@@ -2410,14 +2586,1879 @@
       <c r="U23" s="1">
         <v>33.494</v>
       </c>
-      <c r="V23" s="1">
+      <c r="V23" s="3">
         <v>3035.5</v>
       </c>
       <c r="W23" s="1">
         <v>22597</v>
       </c>
-      <c r="X23" s="1">
+      <c r="X23" s="4">
         <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="1">
+        <v>360</v>
+      </c>
+      <c r="F24" s="1">
+        <v>75</v>
+      </c>
+      <c r="G24" s="1">
+        <v>120</v>
+      </c>
+      <c r="H24" s="1">
+        <v>10</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K24" s="1">
+        <v>150</v>
+      </c>
+      <c r="L24" s="1">
+        <v>150</v>
+      </c>
+      <c r="M24" s="1">
+        <v>18</v>
+      </c>
+      <c r="N24" s="1">
+        <v>3</v>
+      </c>
+      <c r="O24" s="1">
+        <v>2</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="T24" s="1">
+        <v>7</v>
+      </c>
+      <c r="U24" s="1">
+        <v>32</v>
+      </c>
+      <c r="V24" s="3">
+        <v>167.27</v>
+      </c>
+      <c r="W24" s="1">
+        <v>1246</v>
+      </c>
+      <c r="X24" s="4">
+        <v>3.0590000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="1">
+        <v>360</v>
+      </c>
+      <c r="F25" s="1">
+        <v>75</v>
+      </c>
+      <c r="G25" s="1">
+        <v>120</v>
+      </c>
+      <c r="H25" s="1">
+        <v>10</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K25" s="1">
+        <v>150</v>
+      </c>
+      <c r="L25" s="1">
+        <v>150</v>
+      </c>
+      <c r="M25" s="1">
+        <v>18</v>
+      </c>
+      <c r="N25" s="1">
+        <v>3</v>
+      </c>
+      <c r="O25" s="1">
+        <v>2</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="T25" s="1">
+        <v>7</v>
+      </c>
+      <c r="U25" s="1">
+        <v>32</v>
+      </c>
+      <c r="V25" s="3">
+        <v>176.5</v>
+      </c>
+      <c r="W25" s="1">
+        <v>1315</v>
+      </c>
+      <c r="X25" s="4">
+        <v>0.58099999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="1">
+        <v>360</v>
+      </c>
+      <c r="F26" s="1">
+        <v>75</v>
+      </c>
+      <c r="G26" s="1">
+        <v>120</v>
+      </c>
+      <c r="H26" s="1">
+        <v>10</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K26" s="1">
+        <v>150</v>
+      </c>
+      <c r="L26" s="1">
+        <v>150</v>
+      </c>
+      <c r="M26" s="1">
+        <v>18</v>
+      </c>
+      <c r="N26" s="1">
+        <v>3</v>
+      </c>
+      <c r="O26" s="1">
+        <v>2</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="T26" s="1">
+        <v>7</v>
+      </c>
+      <c r="U26" s="1">
+        <v>32</v>
+      </c>
+      <c r="V26" s="3">
+        <v>3153</v>
+      </c>
+      <c r="W26" s="1">
+        <v>23482</v>
+      </c>
+      <c r="X26" s="4">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Y26" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="1">
+        <v>360</v>
+      </c>
+      <c r="F27" s="1">
+        <v>75</v>
+      </c>
+      <c r="G27" s="1">
+        <v>120</v>
+      </c>
+      <c r="H27" s="1">
+        <v>10</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K27" s="1">
+        <v>150</v>
+      </c>
+      <c r="L27" s="1">
+        <v>150</v>
+      </c>
+      <c r="M27" s="1">
+        <v>18</v>
+      </c>
+      <c r="N27" s="1">
+        <v>3</v>
+      </c>
+      <c r="O27" s="1">
+        <v>2</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="T27" s="1">
+        <v>7</v>
+      </c>
+      <c r="U27" s="1">
+        <v>32</v>
+      </c>
+      <c r="V27" s="3">
+        <v>3168.1</v>
+      </c>
+      <c r="W27" s="1">
+        <v>23592</v>
+      </c>
+      <c r="X27" s="4">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="Y27" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="1">
+        <v>360</v>
+      </c>
+      <c r="F28" s="1">
+        <v>75</v>
+      </c>
+      <c r="G28" s="1">
+        <v>120</v>
+      </c>
+      <c r="H28" s="1">
+        <v>10</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K28" s="1">
+        <v>150</v>
+      </c>
+      <c r="L28" s="1">
+        <v>150</v>
+      </c>
+      <c r="M28" s="1">
+        <v>18</v>
+      </c>
+      <c r="N28" s="1">
+        <v>3</v>
+      </c>
+      <c r="O28" s="1">
+        <v>2</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="T28" s="1">
+        <v>7</v>
+      </c>
+      <c r="U28" s="1">
+        <v>32</v>
+      </c>
+      <c r="V28" s="3">
+        <v>3179.3</v>
+      </c>
+      <c r="W28" s="1">
+        <v>23675</v>
+      </c>
+      <c r="X28" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y28" s="2"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="1">
+        <v>360</v>
+      </c>
+      <c r="F29" s="1">
+        <v>75</v>
+      </c>
+      <c r="G29" s="1">
+        <v>120</v>
+      </c>
+      <c r="H29" s="1">
+        <v>10</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K29" s="1">
+        <v>150</v>
+      </c>
+      <c r="L29" s="1">
+        <v>150</v>
+      </c>
+      <c r="M29" s="1">
+        <v>18</v>
+      </c>
+      <c r="N29" s="1">
+        <v>3</v>
+      </c>
+      <c r="O29" s="1">
+        <v>2</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="T29" s="1">
+        <v>7</v>
+      </c>
+      <c r="U29" s="1">
+        <v>32</v>
+      </c>
+      <c r="V29" s="3">
+        <v>3186.2</v>
+      </c>
+      <c r="W29" s="1">
+        <v>23727</v>
+      </c>
+      <c r="X29" s="4">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="Y29" s="2"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="1">
+        <v>360</v>
+      </c>
+      <c r="F30" s="1">
+        <v>75</v>
+      </c>
+      <c r="G30" s="1">
+        <v>120</v>
+      </c>
+      <c r="H30" s="1">
+        <v>10</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K30" s="1">
+        <v>150</v>
+      </c>
+      <c r="L30" s="1">
+        <v>150</v>
+      </c>
+      <c r="M30" s="1">
+        <v>18</v>
+      </c>
+      <c r="N30" s="1">
+        <v>3</v>
+      </c>
+      <c r="O30" s="1">
+        <v>2</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="T30" s="1">
+        <v>7</v>
+      </c>
+      <c r="U30" s="1">
+        <v>32</v>
+      </c>
+      <c r="V30" s="3">
+        <v>3189.4</v>
+      </c>
+      <c r="W30" s="1">
+        <v>23750</v>
+      </c>
+      <c r="X30" s="4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="1">
+        <v>360</v>
+      </c>
+      <c r="F31" s="1">
+        <v>75</v>
+      </c>
+      <c r="G31" s="1">
+        <v>120</v>
+      </c>
+      <c r="H31" s="1">
+        <v>10</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J31" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K31" s="1">
+        <v>150</v>
+      </c>
+      <c r="L31" s="1">
+        <v>150</v>
+      </c>
+      <c r="M31" s="1">
+        <v>18</v>
+      </c>
+      <c r="N31" s="1">
+        <v>3</v>
+      </c>
+      <c r="O31" s="1">
+        <v>2</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="T31" s="1">
+        <v>4</v>
+      </c>
+      <c r="U31" s="1">
+        <v>32</v>
+      </c>
+      <c r="V31" s="3">
+        <v>3277.2</v>
+      </c>
+      <c r="W31" s="1">
+        <v>23774</v>
+      </c>
+      <c r="X31" s="4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="Y31" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="1">
+        <v>360</v>
+      </c>
+      <c r="F32" s="1">
+        <v>75</v>
+      </c>
+      <c r="G32" s="1">
+        <v>120</v>
+      </c>
+      <c r="H32" s="1">
+        <v>10</v>
+      </c>
+      <c r="I32" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J32" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K32" s="1">
+        <v>150</v>
+      </c>
+      <c r="L32" s="1">
+        <v>150</v>
+      </c>
+      <c r="M32" s="1">
+        <v>18</v>
+      </c>
+      <c r="N32" s="1">
+        <v>3</v>
+      </c>
+      <c r="O32" s="1">
+        <v>2</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="T32" s="1">
+        <v>7</v>
+      </c>
+      <c r="U32" s="1">
+        <v>32</v>
+      </c>
+      <c r="V32" s="3">
+        <v>3189</v>
+      </c>
+      <c r="W32" s="1">
+        <v>23746</v>
+      </c>
+      <c r="X32" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="1">
+        <v>360</v>
+      </c>
+      <c r="F33" s="1">
+        <v>75</v>
+      </c>
+      <c r="G33" s="1">
+        <v>120</v>
+      </c>
+      <c r="H33" s="1">
+        <v>10</v>
+      </c>
+      <c r="I33" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J33" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K33" s="1">
+        <v>150</v>
+      </c>
+      <c r="L33" s="1">
+        <v>150</v>
+      </c>
+      <c r="M33" s="1">
+        <v>18</v>
+      </c>
+      <c r="N33" s="1">
+        <v>3</v>
+      </c>
+      <c r="O33" s="1">
+        <v>2</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="T33" s="1">
+        <v>7</v>
+      </c>
+      <c r="U33" s="1">
+        <v>32</v>
+      </c>
+      <c r="V33" s="3">
+        <v>3191.6</v>
+      </c>
+      <c r="W33" s="1">
+        <v>23765</v>
+      </c>
+      <c r="X33" s="4">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="1">
+        <v>360</v>
+      </c>
+      <c r="F34" s="1">
+        <v>75</v>
+      </c>
+      <c r="G34" s="1">
+        <v>120</v>
+      </c>
+      <c r="H34" s="1">
+        <v>10</v>
+      </c>
+      <c r="I34" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J34" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K34" s="1">
+        <v>150</v>
+      </c>
+      <c r="L34" s="1">
+        <v>150</v>
+      </c>
+      <c r="M34" s="1">
+        <v>18</v>
+      </c>
+      <c r="N34" s="1">
+        <v>3</v>
+      </c>
+      <c r="O34" s="1">
+        <v>2</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="T34" s="1">
+        <v>7</v>
+      </c>
+      <c r="U34" s="1">
+        <v>32</v>
+      </c>
+      <c r="V34" s="3">
+        <v>3189.7</v>
+      </c>
+      <c r="W34" s="1">
+        <v>23751</v>
+      </c>
+      <c r="X34" s="4">
+        <v>0.114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="1">
+        <v>360</v>
+      </c>
+      <c r="F35" s="1">
+        <v>75</v>
+      </c>
+      <c r="G35" s="1">
+        <v>120</v>
+      </c>
+      <c r="H35" s="1">
+        <v>10</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J35" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K35" s="1">
+        <v>150</v>
+      </c>
+      <c r="L35" s="1">
+        <v>150</v>
+      </c>
+      <c r="M35" s="1">
+        <v>15</v>
+      </c>
+      <c r="N35" s="1">
+        <v>3</v>
+      </c>
+      <c r="O35" s="1">
+        <v>2</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T35" s="1">
+        <v>2</v>
+      </c>
+      <c r="U35" s="1">
+        <v>33.494</v>
+      </c>
+      <c r="V35" s="3">
+        <v>2947.4</v>
+      </c>
+      <c r="W35" s="1">
+        <v>18289</v>
+      </c>
+      <c r="X35" s="4">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="Y35" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="1">
+        <v>360</v>
+      </c>
+      <c r="F36" s="1">
+        <v>75</v>
+      </c>
+      <c r="G36" s="1">
+        <v>120</v>
+      </c>
+      <c r="H36" s="1">
+        <v>10</v>
+      </c>
+      <c r="I36" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J36" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K36" s="1">
+        <v>150</v>
+      </c>
+      <c r="L36" s="1">
+        <v>150</v>
+      </c>
+      <c r="M36" s="1">
+        <v>18</v>
+      </c>
+      <c r="N36" s="1">
+        <v>3</v>
+      </c>
+      <c r="O36" s="1">
+        <v>2</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="T36" s="1">
+        <v>2</v>
+      </c>
+      <c r="U36" s="1">
+        <v>33.494</v>
+      </c>
+      <c r="V36" s="3">
+        <v>2960.8</v>
+      </c>
+      <c r="W36" s="1">
+        <v>22047</v>
+      </c>
+      <c r="X36" s="4">
+        <v>6.2E-2</v>
+      </c>
+      <c r="Y36" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="1">
+        <v>360</v>
+      </c>
+      <c r="F37" s="1">
+        <v>75</v>
+      </c>
+      <c r="G37" s="1">
+        <v>120</v>
+      </c>
+      <c r="H37" s="1">
+        <v>10</v>
+      </c>
+      <c r="I37" s="1">
+        <v>1400</v>
+      </c>
+      <c r="J37" s="1">
+        <v>1400</v>
+      </c>
+      <c r="K37" s="1">
+        <v>150</v>
+      </c>
+      <c r="L37" s="1">
+        <v>150</v>
+      </c>
+      <c r="M37" s="1">
+        <v>21</v>
+      </c>
+      <c r="N37" s="1">
+        <v>3</v>
+      </c>
+      <c r="O37" s="1">
+        <v>2</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="T37" s="1">
+        <v>2</v>
+      </c>
+      <c r="U37" s="1">
+        <v>33.494</v>
+      </c>
+      <c r="V37" s="3">
+        <v>2974.8</v>
+      </c>
+      <c r="W37" s="1">
+        <v>25844</v>
+      </c>
+      <c r="X37" s="4">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="Y37" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="1">
+        <v>360</v>
+      </c>
+      <c r="F38" s="1">
+        <v>75</v>
+      </c>
+      <c r="G38" s="1">
+        <v>120</v>
+      </c>
+      <c r="H38" s="1">
+        <v>10</v>
+      </c>
+      <c r="I38" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K38" s="1">
+        <v>150</v>
+      </c>
+      <c r="L38" s="1">
+        <v>150</v>
+      </c>
+      <c r="M38" s="1">
+        <v>18</v>
+      </c>
+      <c r="N38" s="1">
+        <v>3</v>
+      </c>
+      <c r="O38" s="1">
+        <v>2</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T38" s="1">
+        <v>2</v>
+      </c>
+      <c r="U38" s="1">
+        <v>32</v>
+      </c>
+      <c r="V38" s="3">
+        <v>3196.7</v>
+      </c>
+      <c r="W38" s="1">
+        <v>23803</v>
+      </c>
+      <c r="X38" s="4">
+        <v>2.4E-2</v>
+      </c>
+      <c r="Y38" s="2"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="1">
+        <v>360</v>
+      </c>
+      <c r="F39" s="1">
+        <v>75</v>
+      </c>
+      <c r="G39" s="1">
+        <v>120</v>
+      </c>
+      <c r="H39" s="1">
+        <v>10</v>
+      </c>
+      <c r="I39" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J39" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K39" s="1">
+        <v>150</v>
+      </c>
+      <c r="L39" s="1">
+        <v>150</v>
+      </c>
+      <c r="M39" s="1">
+        <v>18</v>
+      </c>
+      <c r="N39" s="1">
+        <v>3</v>
+      </c>
+      <c r="O39" s="1">
+        <v>2</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="T39" s="1">
+        <v>2</v>
+      </c>
+      <c r="U39" s="1">
+        <v>32</v>
+      </c>
+      <c r="V39" s="3">
+        <v>3201.6</v>
+      </c>
+      <c r="W39" s="1">
+        <v>23839</v>
+      </c>
+      <c r="X39" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="1">
+        <v>360</v>
+      </c>
+      <c r="F40" s="1">
+        <v>75</v>
+      </c>
+      <c r="G40" s="1">
+        <v>120</v>
+      </c>
+      <c r="H40" s="1">
+        <v>10</v>
+      </c>
+      <c r="I40" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J40" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K40" s="1">
+        <v>150</v>
+      </c>
+      <c r="L40" s="1">
+        <v>150</v>
+      </c>
+      <c r="M40" s="1">
+        <v>18</v>
+      </c>
+      <c r="N40" s="1">
+        <v>3</v>
+      </c>
+      <c r="O40" s="1">
+        <v>2</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="T40" s="1">
+        <v>2</v>
+      </c>
+      <c r="U40" s="1">
+        <v>32</v>
+      </c>
+      <c r="V40" s="3">
+        <v>3200.7</v>
+      </c>
+      <c r="W40" s="1">
+        <v>23832</v>
+      </c>
+      <c r="X40" s="4">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="1">
+        <v>360</v>
+      </c>
+      <c r="F41" s="1">
+        <v>75</v>
+      </c>
+      <c r="G41" s="1">
+        <v>120</v>
+      </c>
+      <c r="H41" s="1">
+        <v>10</v>
+      </c>
+      <c r="I41" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J41" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K41" s="1">
+        <v>150</v>
+      </c>
+      <c r="L41" s="1">
+        <v>150</v>
+      </c>
+      <c r="M41" s="1">
+        <v>18</v>
+      </c>
+      <c r="N41" s="1">
+        <v>3</v>
+      </c>
+      <c r="O41" s="1">
+        <v>2</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="T41" s="1">
+        <v>2</v>
+      </c>
+      <c r="U41" s="1">
+        <v>32</v>
+      </c>
+      <c r="V41" s="3">
+        <v>3200.2</v>
+      </c>
+      <c r="W41" s="1">
+        <v>23829</v>
+      </c>
+      <c r="X41" s="4">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" s="1">
+        <v>360</v>
+      </c>
+      <c r="F42" s="1">
+        <v>75</v>
+      </c>
+      <c r="G42" s="1">
+        <v>120</v>
+      </c>
+      <c r="H42" s="1">
+        <v>10</v>
+      </c>
+      <c r="I42" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J42" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K42" s="1">
+        <v>150</v>
+      </c>
+      <c r="L42" s="1">
+        <v>150</v>
+      </c>
+      <c r="M42" s="1">
+        <v>18</v>
+      </c>
+      <c r="N42" s="1">
+        <v>3</v>
+      </c>
+      <c r="O42" s="1">
+        <v>2</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S42" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="T42" s="1">
+        <v>2</v>
+      </c>
+      <c r="U42" s="1">
+        <v>32</v>
+      </c>
+      <c r="V42" s="3">
+        <v>3193.8</v>
+      </c>
+      <c r="W42" s="1">
+        <v>23781</v>
+      </c>
+      <c r="X42" s="4">
+        <v>0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="1">
+        <v>360</v>
+      </c>
+      <c r="F43" s="1">
+        <v>75</v>
+      </c>
+      <c r="G43" s="1">
+        <v>120</v>
+      </c>
+      <c r="H43" s="1">
+        <v>10</v>
+      </c>
+      <c r="I43" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J43" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K43" s="1">
+        <v>150</v>
+      </c>
+      <c r="L43" s="1">
+        <v>150</v>
+      </c>
+      <c r="M43" s="1">
+        <v>18</v>
+      </c>
+      <c r="N43" s="1">
+        <v>3</v>
+      </c>
+      <c r="O43" s="1">
+        <v>2</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S43" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="T43" s="1">
+        <v>2</v>
+      </c>
+      <c r="U43" s="1">
+        <v>32</v>
+      </c>
+      <c r="V43" s="3">
+        <v>3196</v>
+      </c>
+      <c r="W43" s="1">
+        <v>23798</v>
+      </c>
+      <c r="X43" s="4">
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="1">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="1">
+        <v>360</v>
+      </c>
+      <c r="F44" s="1">
+        <v>75</v>
+      </c>
+      <c r="G44" s="1">
+        <v>120</v>
+      </c>
+      <c r="H44" s="1">
+        <v>10</v>
+      </c>
+      <c r="I44" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J44" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K44" s="1">
+        <v>150</v>
+      </c>
+      <c r="L44" s="1">
+        <v>150</v>
+      </c>
+      <c r="M44" s="1">
+        <v>18</v>
+      </c>
+      <c r="N44" s="1">
+        <v>3</v>
+      </c>
+      <c r="O44" s="1">
+        <v>2</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S44" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="T44" s="1">
+        <v>2</v>
+      </c>
+      <c r="U44" s="1">
+        <v>32</v>
+      </c>
+      <c r="V44" s="3">
+        <v>3195.8</v>
+      </c>
+      <c r="W44" s="1">
+        <v>23795</v>
+      </c>
+      <c r="X44" s="4">
+        <v>9.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E45" s="1">
+        <v>360</v>
+      </c>
+      <c r="F45" s="1">
+        <v>75</v>
+      </c>
+      <c r="G45" s="1">
+        <v>120</v>
+      </c>
+      <c r="H45" s="1">
+        <v>10</v>
+      </c>
+      <c r="I45" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J45" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K45" s="1">
+        <v>150</v>
+      </c>
+      <c r="L45" s="1">
+        <v>150</v>
+      </c>
+      <c r="M45" s="1">
+        <v>18</v>
+      </c>
+      <c r="N45" s="1">
+        <v>3</v>
+      </c>
+      <c r="O45" s="1">
+        <v>2</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="T45" s="1">
+        <v>2</v>
+      </c>
+      <c r="U45" s="1">
+        <v>32</v>
+      </c>
+      <c r="V45" s="3">
+        <v>3193</v>
+      </c>
+      <c r="W45" s="1">
+        <v>23774</v>
+      </c>
+      <c r="X45" s="4">
+        <v>8.6999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E46" s="1">
+        <v>360</v>
+      </c>
+      <c r="F46" s="1">
+        <v>75</v>
+      </c>
+      <c r="G46" s="1">
+        <v>120</v>
+      </c>
+      <c r="H46" s="1">
+        <v>10</v>
+      </c>
+      <c r="I46" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J46" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K46" s="1">
+        <v>150</v>
+      </c>
+      <c r="L46" s="1">
+        <v>150</v>
+      </c>
+      <c r="M46" s="1">
+        <v>18</v>
+      </c>
+      <c r="N46" s="1">
+        <v>3</v>
+      </c>
+      <c r="O46" s="1">
+        <v>2</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="T46" s="1">
+        <v>2</v>
+      </c>
+      <c r="U46" s="1">
+        <v>32</v>
+      </c>
+      <c r="V46" s="3">
+        <v>3194.7</v>
+      </c>
+      <c r="W46" s="1">
+        <v>23787</v>
+      </c>
+      <c r="X46" s="4">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E47" s="1">
+        <v>360</v>
+      </c>
+      <c r="F47" s="1">
+        <v>75</v>
+      </c>
+      <c r="G47" s="1">
+        <v>120</v>
+      </c>
+      <c r="H47" s="1">
+        <v>10</v>
+      </c>
+      <c r="I47" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J47" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K47" s="1">
+        <v>150</v>
+      </c>
+      <c r="L47" s="1">
+        <v>150</v>
+      </c>
+      <c r="M47" s="1">
+        <v>18</v>
+      </c>
+      <c r="N47" s="1">
+        <v>3</v>
+      </c>
+      <c r="O47" s="1">
+        <v>2</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="T47" s="1">
+        <v>2</v>
+      </c>
+      <c r="U47" s="1">
+        <v>32</v>
+      </c>
+      <c r="V47" s="3">
+        <v>3197.6</v>
+      </c>
+      <c r="W47" s="1">
+        <v>23808</v>
+      </c>
+      <c r="X47" s="1">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E48" s="1">
+        <v>360</v>
+      </c>
+      <c r="F48" s="1">
+        <v>75</v>
+      </c>
+      <c r="G48" s="1">
+        <v>120</v>
+      </c>
+      <c r="H48" s="1">
+        <v>10</v>
+      </c>
+      <c r="I48" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J48" s="1">
+        <v>1200</v>
+      </c>
+      <c r="K48" s="1">
+        <v>150</v>
+      </c>
+      <c r="L48" s="1">
+        <v>150</v>
+      </c>
+      <c r="M48" s="1">
+        <v>18</v>
+      </c>
+      <c r="N48" s="1">
+        <v>3</v>
+      </c>
+      <c r="O48" s="1">
+        <v>2</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="T48" s="1">
+        <v>2</v>
+      </c>
+      <c r="U48" s="1">
+        <v>33.494</v>
+      </c>
+      <c r="V48" s="3">
+        <v>3060.2</v>
+      </c>
+      <c r="Y48" s="2" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>